<commit_message>
Fix table report for requirements
</commit_message>
<xml_diff>
--- a/Documentation/Final Report/Image and media content/FYP - List of requirements with priority.xlsx
+++ b/Documentation/Final Report/Image and media content/FYP - List of requirements with priority.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shouyi Cui\Dropbox\FYP management\Official Work [On GitHub]\Contactless-Voucher\Documentation\Final Report\Image and media content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB8BBFC-7F3C-4EB3-AC62-76DDEE451E16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B4F0A-49DC-439F-9B27-3872C913FD98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{F3108A73-4E7E-41DB-BA0F-03CFD0B1EC69}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -197,13 +197,19 @@
     <t>Web App shall be working with Android NFC</t>
   </si>
   <si>
-    <t>User shall be able see the home page without registering and redirected to it if not logged in</t>
-  </si>
-  <si>
     <t>Web App shall have different login depending on customer or cashier/retailer</t>
   </si>
   <si>
     <t>Web App shall have different content depending on customer or cashier/retailer</t>
+  </si>
+  <si>
+    <t>User should be redirected to homepage if not logged in</t>
+  </si>
+  <si>
+    <t>Web App shall display the home page for users not registered</t>
+  </si>
+  <si>
+    <t>NFR10</t>
   </si>
 </sst>
 </file>
@@ -235,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -243,15 +249,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -289,8 +307,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D48AFB6-42B4-487D-A884-9AE3C3AF3084}" name="Tabella2" displayName="Tabella2" ref="A19:C28" totalsRowShown="0">
-  <autoFilter ref="A19:C28" xr:uid="{3A9FA6C3-514F-4664-88BC-83136025C315}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D48AFB6-42B4-487D-A884-9AE3C3AF3084}" name="Tabella2" displayName="Tabella2" ref="A19:C29" totalsRowShown="0">
+  <autoFilter ref="A19:C29" xr:uid="{3A9FA6C3-514F-4664-88BC-83136025C315}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BE9B8702-348C-408D-91C6-9BF33F49B0C8}" name="ID"/>
     <tableColumn id="2" xr3:uid="{4EDCDA5B-7F4C-43BE-BF6A-BE8C8AA278DB}" name="Description"/>
@@ -599,14 +617,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195B3B82-AED9-4514-AACA-41DE7CA4894D}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,7 +644,7 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -637,7 +655,7 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -648,7 +666,7 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -815,8 +833,8 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>47</v>
+      <c r="B20" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>16</v>
@@ -827,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>16</v>
@@ -838,7 +856,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>16</v>
@@ -849,7 +867,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>16</v>
@@ -860,10 +878,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -871,10 +889,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -882,9 +900,9 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -893,10 +911,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,14 +922,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C29" s="1"/>
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>

</xml_diff>